<commit_message>
crypto graphs updated for new sentiment data
yeee
</commit_message>
<xml_diff>
--- a/crypto prices.xlsx
+++ b/crypto prices.xlsx
@@ -19,28 +19,6 @@
     <sheet name="LTC" sheetId="4" r:id="rId5"/>
     <sheet name="XRP" sheetId="5" r:id="rId6"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$C$13:$C$22</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$C$13:$C$22</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$D$13:$D$22</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$E$1</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$E$13:$E$22</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$F$1</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$F$13:$F$22</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$G$1</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$G$13:$G$22</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$D$13:$D$22</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$E$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$E$13:$E$22</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$F$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$F$13:$F$22</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$G$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$G$13:$G$22</definedName>
-  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -176,7 +154,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -197,6 +175,833 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>LTC</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs. Positive Sentiment</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LTC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$14:$L$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4.0979510244877577</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-19.987197951672272</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.1400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-8.454527826255573</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-4.6600296547341724</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17.307265052210617</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-2.784090909090907</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.6169881161114326</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-5.5598159509202434</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1250-4D8A-8E9F-B71E5CE56947}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>positive</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$31:$H$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-24.97056030808978</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.2495798459014451</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-3.7632099286053879</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-5.0274123623505096</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.605135880283953</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-20.774713336837848</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.549467138836956</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.4185424544875267</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1250-4D8A-8E9F-B71E5CE56947}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="405163472"/>
+        <c:axId val="405158552"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="405163472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="405158552"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="405158552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="405163472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Namecoin</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs. Positive Sentiment</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Namecoin</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$14:$M$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>6.7164179104477499</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.5944055944055995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-15.894039735099337</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-10.236220472440953</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-19.298245614035078</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.8695652173912967</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24.229979466119094</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-4.958677685950418</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0103-48C6-A8C0-6F420DD77D8F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>positive</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$31:$H$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-24.97056030808978</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.2495798459014451</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-3.7632099286053879</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-5.0274123623505096</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.605135880283953</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-20.774713336837848</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.549467138836956</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.4185424544875267</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.569477247124816</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0103-48C6-A8C0-6F420DD77D8F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="416620184"/>
+        <c:axId val="416622152"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="416620184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="416622152"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="416622152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="416620184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -302,6 +1107,75 @@
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
               <c15:ser>
+                <c:idx val="5"/>
+                <c:order val="5"/>
+                <c:tx>
+                  <c:v>Positive</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent6"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$E$30:$E$39</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>-24.97056030808978</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>-25.908113064972667</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>-28.696346310402696</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>-32.281075010801111</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>-21.713444749569049</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>-37.977252184131267</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>-27.712817915740349</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>-26.687393548722426</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>-18.938634290580481</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-FB12-40FB-A401-165514E880C2}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
                 <c:idx val="6"/>
                 <c:order val="6"/>
                 <c:tx>
@@ -321,8 +1195,8 @@
                 <c:invertIfNegative val="0"/>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$C$30:$C$40</c15:sqref>
                         </c15:formulaRef>
@@ -364,7 +1238,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-FB12-40FB-A401-165514E880C2}"/>
                   </c:ext>
@@ -392,7 +1266,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$F$30:$F$39</c15:sqref>
@@ -435,78 +1309,9 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-FB12-40FB-A401-165514E880C2}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredBarSeries>
-            <c15:filteredBarSeries>
-              <c15:ser>
-                <c:idx val="5"/>
-                <c:order val="5"/>
-                <c:tx>
-                  <c:v>Positive</c:v>
-                </c:tx>
-                <c:spPr>
-                  <a:solidFill>
-                    <a:schemeClr val="accent6"/>
-                  </a:solidFill>
-                  <a:ln>
-                    <a:noFill/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:invertIfNegative val="0"/>
-                <c:val>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$E$30:$E$39</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="10"/>
-                      <c:pt idx="0">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>-15.135474708438727</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>-20.266940439935659</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>-19.549463796069759</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>-23.284421734026566</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>-12.098634223109428</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>-26.888409952280316</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>-18.353860267482787</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>-16.961796688104396</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>-8.6735264199935589</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:val>
-                <c:extLst>
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000000-FB12-40FB-A401-165514E880C2}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -1160,7 +1965,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1621,31 +2426,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.44654044878997201</c:v>
+                  <c:v>0.507860274</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.37895443210041702</c:v>
+                  <c:v>0.381044718</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.35604036199348699</c:v>
+                  <c:v>0.37628326000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.35924418541896902</c:v>
+                  <c:v>0.36212293099999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.3425660874807</c:v>
+                  <c:v>0.34391751799999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.39251515323264202</c:v>
+                  <c:v>0.397586314</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.32647282231657199</c:v>
+                  <c:v>0.31498889699999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.36458303878127002</c:v>
+                  <c:v>0.36711788099999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.37079916573606803</c:v>
+                  <c:v>0.37232560399999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1888,6 +2693,7 @@
         <c:axId val="416315088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="0.5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
@@ -1951,6 +2757,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="416315088"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2032,7 +2839,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2216,28 +3023,28 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-15.135474708438727</c:v>
+                  <c:v>-24.97056030808978</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-6.0466557891736592</c:v>
+                  <c:v>-1.2495798459014451</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.89984837885897895</c:v>
+                  <c:v>-3.7632099286053879</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-4.6425519507902866</c:v>
+                  <c:v>-5.0274123623505096</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14.580855366997215</c:v>
+                  <c:v>15.605135880283953</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-16.825421992543312</c:v>
+                  <c:v>-20.774713336837848</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.67331975576931</c:v>
+                  <c:v>16.549467138836956</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.7049961993781462</c:v>
+                  <c:v>1.4185424544875267</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2443,7 +3250,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2615,39 +3422,36 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$31:$H$40</c:f>
+              <c:f>Sheet1!$H$31:$H$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-15.135474708438727</c:v>
+                  <c:v>-24.97056030808978</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-6.0466557891736592</c:v>
+                  <c:v>-1.2495798459014451</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.89984837885897895</c:v>
+                  <c:v>-3.7632099286053879</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-4.6425519507902866</c:v>
+                  <c:v>-5.0274123623505096</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14.580855366997215</c:v>
+                  <c:v>15.605135880283953</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-16.825421992543312</c:v>
+                  <c:v>-20.774713336837848</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.67331975576931</c:v>
+                  <c:v>16.549467138836956</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.7049961993781462</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9.9812736036444392</c:v>
+                  <c:v>1.4185424544875267</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2853,7 +3657,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3025,39 +3829,36 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$31:$H$40</c:f>
+              <c:f>Sheet1!$H$31:$H$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-15.135474708438727</c:v>
+                  <c:v>-24.97056030808978</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-6.0466557891736592</c:v>
+                  <c:v>-1.2495798459014451</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.89984837885897895</c:v>
+                  <c:v>-3.7632099286053879</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-4.6425519507902866</c:v>
+                  <c:v>-5.0274123623505096</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14.580855366997215</c:v>
+                  <c:v>15.605135880283953</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-16.825421992543312</c:v>
+                  <c:v>-20.774713336837848</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.67331975576931</c:v>
+                  <c:v>16.549467138836956</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.7049961993781462</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9.9812736036444392</c:v>
+                  <c:v>1.4185424544875267</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3184,836 +3985,6 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="642639696"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>LTC</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> vs. Positive Sentiment</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$L$13</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>LTC</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$L$14:$L$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>4.0979510244877577</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-19.987197951672272</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.1400000000000006</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-8.454527826255573</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-4.6600296547341724</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>17.307265052210617</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-2.784090909090907</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.6169881161114326</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-5.5598159509202434</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1250-4D8A-8E9F-B71E5CE56947}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$H$30</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>positive</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$H$31:$H$40</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-15.135474708438727</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-6.0466557891736592</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.89984837885897895</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-4.6425519507902866</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>14.580855366997215</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-16.825421992543312</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>11.67331975576931</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.7049961993781462</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9.9812736036444392</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-1250-4D8A-8E9F-B71E5CE56947}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="405163472"/>
-        <c:axId val="405158552"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="405163472"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="405158552"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="405158552"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="405163472"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Namecoin</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> vs. Positive Sentiment</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$M$13</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Namecoin</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$M$14:$M$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>6.7164179104477499</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.5944055944055995</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-15.894039735099337</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-10.236220472440953</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-19.298245614035078</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.8695652173912967</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>24.229979466119094</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-4.958677685950418</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0103-48C6-A8C0-6F420DD77D8F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$H$30</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>positive</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$H$31:$H$40</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-15.135474708438727</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-6.0466557891736592</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.89984837885897895</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-4.6425519507902866</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>14.580855366997215</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-16.825421992543312</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>11.67331975576931</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.7049961993781462</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9.9812736036444392</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0103-48C6-A8C0-6F420DD77D8F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="416620184"/>
-        <c:axId val="416622152"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="416620184"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="416622152"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="416622152"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="416620184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4890,7 +4861,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="322">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -4998,6 +4969,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -5008,6 +4984,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -5039,6 +5020,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5094,23 +5078,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -5280,17 +5263,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -5359,20 +5331,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -5922,7 +5893,7 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="322">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -6030,11 +6001,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -6045,11 +6011,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -6081,9 +6042,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6139,22 +6097,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -6324,6 +6283,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -6392,19 +6362,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -7987,6 +7958,78 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>21167</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>51857</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>296333</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>128057</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B414A5E9-E04E-46B4-89FB-EBDE067A6225}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>51857</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>42334</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>128057</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C25BC25-005F-4E43-9B3C-ECE7AA51623B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
@@ -8017,7 +8060,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -8053,78 +8096,6 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>74084</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>83607</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>349251</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>159807</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABC03A0B-09EC-49F2-8FE1-8CF261A23670}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>370417</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>31750</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3269F408-E56F-4169-9203-272482437FEB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
@@ -8133,23 +8104,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>545040</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>125941</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>402167</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>38</xdr:col>
-      <xdr:colOff>206374</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>11641</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 7">
+        <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A1AADF1-491B-4080-B5ED-05BC6237C344}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABC03A0B-09EC-49F2-8FE1-8CF261A23670}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8169,23 +8140,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>21167</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>51857</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>105833</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>30690</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>39</xdr:col>
-      <xdr:colOff>296333</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>128057</xdr:rowOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>106890</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="Chart 8">
+        <xdr:cNvPr id="7" name="Chart 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B414A5E9-E04E-46B4-89FB-EBDE067A6225}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3269F408-E56F-4169-9203-272482437FEB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8205,23 +8176,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>178857</xdr:rowOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>407457</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>41274</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>40</xdr:col>
-      <xdr:colOff>275167</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>64557</xdr:rowOff>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>68790</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>117474</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Chart 9">
+        <xdr:cNvPr id="8" name="Chart 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C25BC25-005F-4E43-9B3C-ECE7AA51623B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A1AADF1-491B-4080-B5ED-05BC6237C344}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8784,10 +8755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B84E35BA-E282-44AF-A38C-C8FD92A2D4C7}">
-  <dimension ref="A1:M40"/>
+  <dimension ref="A1:M60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="S20" sqref="S20"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AT21" sqref="AT21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9537,9 +9508,9 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>0.44654044878997201</v>
-      </c>
-      <c r="B30">
+        <v>0.507860274</v>
+      </c>
+      <c r="B30" s="1">
         <v>0.31284419774950101</v>
       </c>
       <c r="C30" s="1">
@@ -9562,20 +9533,20 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>0.37895443210041702</v>
-      </c>
-      <c r="B31">
+        <v>0.381044718</v>
+      </c>
+      <c r="B31" s="1">
         <v>0.26880712613944302</v>
       </c>
       <c r="C31" s="1">
         <v>0.18222684774608916</v>
       </c>
       <c r="E31" s="1">
-        <f t="shared" ref="E31:E39" si="7">100*(A31-$A$30)/$A$30</f>
-        <v>-15.135474708438727</v>
+        <f>100*(A31-$A$30)/$A$30</f>
+        <v>-24.97056030808978</v>
       </c>
       <c r="F31" s="1">
-        <f t="shared" ref="F31:F39" si="8">100*(B31-$B$30)/$B$30</f>
+        <f t="shared" ref="F31:F39" si="7">100*(B31-$B$30)/$B$30</f>
         <v>-14.076358752007005</v>
       </c>
       <c r="H31" s="1">
@@ -9588,218 +9559,277 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>0.35604036199348699</v>
-      </c>
-      <c r="B32">
+        <v>0.37628326000000001</v>
+      </c>
+      <c r="B32" s="1">
         <v>0.27579147882032401</v>
       </c>
       <c r="C32" s="1">
         <v>0.23131867541201884</v>
       </c>
       <c r="E32" s="1">
+        <f>100*(A32-$A$30)/$A$30</f>
+        <v>-25.908113064972667</v>
+      </c>
+      <c r="F32" s="1">
         <f t="shared" si="7"/>
-        <v>-20.266940439935659</v>
-      </c>
-      <c r="F32" s="1">
-        <f t="shared" si="8"/>
         <v>-11.843824880155092</v>
       </c>
       <c r="H32" s="1">
-        <v>-15.135474708438727</v>
+        <f>100*(A31-A30)/A30</f>
+        <v>-24.97056030808978</v>
       </c>
       <c r="I32" s="1">
-        <f t="shared" ref="I32:I39" si="9">100*(B32-B31)/B31</f>
+        <f t="shared" ref="I32:I39" si="8">100*(B32-B31)/B31</f>
         <v>2.598276608655782</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>0.35924418541896902</v>
-      </c>
-      <c r="B33">
+        <v>0.36212293099999998</v>
+      </c>
+      <c r="B33" s="1">
         <v>0.286121949138606</v>
       </c>
       <c r="C33" s="1">
         <v>0.1829328187614872</v>
       </c>
       <c r="E33" s="1">
+        <f>100*(A33-$A$30)/$A$30</f>
+        <v>-28.696346310402696</v>
+      </c>
+      <c r="F33" s="1">
         <f t="shared" si="7"/>
-        <v>-19.549463796069759</v>
-      </c>
-      <c r="F33" s="1">
+        <v>-8.5417114343581044</v>
+      </c>
+      <c r="H33" s="1">
+        <f>100*(A32-A31)/A31</f>
+        <v>-1.2495798459014451</v>
+      </c>
+      <c r="I33" s="1">
         <f t="shared" si="8"/>
-        <v>-8.5417114343581044</v>
-      </c>
-      <c r="H33" s="1">
-        <v>-6.0466557891736592</v>
-      </c>
-      <c r="I33" s="1">
-        <f t="shared" si="9"/>
         <v>3.7457539886546725</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>0.3425660874807</v>
-      </c>
-      <c r="B34">
+        <v>0.34391751799999998</v>
+      </c>
+      <c r="B34" s="1">
         <v>0.24396229335314101</v>
       </c>
       <c r="C34" s="1">
         <v>0.22066292044278768</v>
       </c>
       <c r="E34" s="1">
+        <f>100*(A34-$A$30)/$A$30</f>
+        <v>-32.281075010801111</v>
+      </c>
+      <c r="F34" s="1">
         <f t="shared" si="7"/>
-        <v>-23.284421734026566</v>
-      </c>
-      <c r="F34" s="1">
+        <v>-22.017958105623794</v>
+      </c>
+      <c r="H34" s="1">
+        <f>100*(A33-A32)/A32</f>
+        <v>-3.7632099286053879</v>
+      </c>
+      <c r="I34" s="1">
         <f t="shared" si="8"/>
-        <v>-22.017958105623794</v>
-      </c>
-      <c r="H34" s="1">
-        <v>0.89984837885897895</v>
-      </c>
-      <c r="I34" s="1">
-        <f t="shared" si="9"/>
         <v>-14.734855509124744</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>0.39251515323264202</v>
-      </c>
-      <c r="B35">
+        <v>0.397586314</v>
+      </c>
+      <c r="B35" s="1">
         <v>0.27244341119947202</v>
       </c>
       <c r="C35" s="1">
         <v>0.22055771555147113</v>
       </c>
       <c r="E35" s="1">
+        <f>100*(A35-$A$30)/$A$30</f>
+        <v>-21.713444749569049</v>
+      </c>
+      <c r="F35" s="1">
         <f t="shared" si="7"/>
-        <v>-12.098634223109428</v>
-      </c>
-      <c r="F35" s="1">
+        <v>-12.914027762272422</v>
+      </c>
+      <c r="H35" s="1">
+        <f>100*(A34-A33)/A33</f>
+        <v>-5.0274123623505096</v>
+      </c>
+      <c r="I35" s="1">
         <f t="shared" si="8"/>
-        <v>-12.914027762272422</v>
-      </c>
-      <c r="H35" s="1">
-        <v>-4.6425519507902866</v>
-      </c>
-      <c r="I35" s="1">
-        <f t="shared" si="9"/>
         <v>11.674393388778295</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>0.32647282231657199</v>
-      </c>
-      <c r="B36">
+        <v>0.31498889699999999</v>
+      </c>
+      <c r="B36" s="1">
         <v>0.23918579930074099</v>
       </c>
       <c r="C36" s="1">
         <v>0.18465063188226011</v>
       </c>
       <c r="E36" s="1">
+        <f>100*(A36-$A$30)/$A$30</f>
+        <v>-37.977252184131267</v>
+      </c>
+      <c r="F36" s="1">
         <f t="shared" si="7"/>
-        <v>-26.888409952280316</v>
-      </c>
-      <c r="F36" s="1">
+        <v>-23.5447545387239</v>
+      </c>
+      <c r="H36" s="1">
+        <f>100*(A35-A34)/A34</f>
+        <v>15.605135880283953</v>
+      </c>
+      <c r="I36" s="1">
         <f t="shared" si="8"/>
-        <v>-23.5447545387239</v>
-      </c>
-      <c r="H36" s="1">
-        <v>14.580855366997215</v>
-      </c>
-      <c r="I36" s="1">
-        <f t="shared" si="9"/>
         <v>-12.207163224212147</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>0.36458303878127002</v>
-      </c>
-      <c r="B37">
+        <v>0.36711788099999998</v>
+      </c>
+      <c r="B37" s="1">
         <v>0.30668343477203502</v>
       </c>
       <c r="C37" s="1">
         <v>0.17026905959478697</v>
       </c>
       <c r="E37" s="1">
+        <f>100*(A37-$A$30)/$A$30</f>
+        <v>-27.712817915740349</v>
+      </c>
+      <c r="F37" s="1">
         <f t="shared" si="7"/>
-        <v>-18.353860267482787</v>
-      </c>
-      <c r="F37" s="1">
+        <v>-1.9692751285734242</v>
+      </c>
+      <c r="H37" s="1">
+        <f>100*(A36-A35)/A35</f>
+        <v>-20.774713336837848</v>
+      </c>
+      <c r="I37" s="1">
         <f t="shared" si="8"/>
-        <v>-1.9692751285734242</v>
-      </c>
-      <c r="H37" s="1">
-        <v>-16.825421992543312</v>
-      </c>
-      <c r="I37" s="1">
-        <f t="shared" si="9"/>
         <v>28.219750365039719</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>0.37079916573606803</v>
-      </c>
-      <c r="B38">
+        <v>0.37232560399999998</v>
+      </c>
+      <c r="B38" s="1">
         <v>0.20294047927381201</v>
       </c>
       <c r="C38" s="1">
         <v>0.2429858784813918</v>
       </c>
       <c r="E38" s="1">
+        <f>100*(A38-$A$30)/$A$30</f>
+        <v>-26.687393548722426</v>
+      </c>
+      <c r="F38" s="1">
         <f t="shared" si="7"/>
-        <v>-16.961796688104396</v>
-      </c>
-      <c r="F38" s="1">
+        <v>-35.130496031667029</v>
+      </c>
+      <c r="H38" s="1">
+        <f>100*(A37-A36)/A36</f>
+        <v>16.549467138836956</v>
+      </c>
+      <c r="I38" s="1">
         <f t="shared" si="8"/>
-        <v>-35.130496031667029</v>
-      </c>
-      <c r="H38" s="1">
-        <v>11.67331975576931</v>
-      </c>
-      <c r="I38" s="1">
-        <f t="shared" si="9"/>
         <v>-33.827374985328952</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>0.40780964498821598</v>
-      </c>
-      <c r="B39">
+        <v>0.41167847400000002</v>
+      </c>
+      <c r="B39" s="1">
         <v>0.23676164402726799</v>
       </c>
       <c r="C39" s="1">
         <v>0.30702976918123481</v>
       </c>
       <c r="E39" s="1">
+        <f>100*(A39-$A$30)/$A$30</f>
+        <v>-18.938634290580481</v>
+      </c>
+      <c r="F39" s="1">
         <f t="shared" si="7"/>
-        <v>-8.6735264199935589</v>
-      </c>
-      <c r="F39" s="1">
+        <v>-24.319630752159082</v>
+      </c>
+      <c r="H39" s="1">
+        <f>100*(A38-A37)/A37</f>
+        <v>1.4185424544875267</v>
+      </c>
+      <c r="I39" s="1">
         <f t="shared" si="8"/>
-        <v>-24.319630752159082</v>
-      </c>
-      <c r="H39" s="1">
-        <v>1.7049961993781462</v>
-      </c>
-      <c r="I39" s="1">
-        <f t="shared" si="9"/>
         <v>16.665558726617412</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40"/>
-      <c r="B40"/>
+      <c r="A40">
+        <v>0.33984150000000002</v>
+      </c>
       <c r="H40" s="1">
-        <v>9.9812736036444392</v>
-      </c>
+        <f>100*(A39-A38)/A38</f>
+        <v>10.569477247124816</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H41" s="1">
+        <f>100*(A40-A39)/A39</f>
+        <v>-17.449776594342893</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C50" s="3"/>
+      <c r="D50"/>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C51" s="3"/>
+      <c r="D51"/>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C52" s="3"/>
+      <c r="D52"/>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C53" s="3"/>
+      <c r="D53"/>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C54" s="3"/>
+      <c r="D54"/>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C55" s="3"/>
+      <c r="D55"/>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C56" s="3"/>
+      <c r="D56"/>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C57" s="3"/>
+      <c r="D57"/>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C58" s="3"/>
+      <c r="D58"/>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C59" s="3"/>
+      <c r="D59"/>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B60"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>